<commit_message>
Added more text to the documentation file
</commit_message>
<xml_diff>
--- a/data/Crop Rotation Sample Template.xlsx
+++ b/data/Crop Rotation Sample Template.xlsx
@@ -5,21 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\Documents\Documentation\Gardening Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\Documents\Rwork\CropRotationWithOMPR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9312" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9312"/>
   </bookViews>
   <sheets>
     <sheet name="Farmland" sheetId="3" r:id="rId1"/>
     <sheet name="Crops" sheetId="1" r:id="rId2"/>
     <sheet name="Demand" sheetId="4" r:id="rId3"/>
-    <sheet name="Model" sheetId="5" r:id="rId4"/>
-    <sheet name="Constraints" sheetId="2" r:id="rId5"/>
-    <sheet name="Land Use Constraints" sheetId="6" r:id="rId6"/>
-    <sheet name="Demand Constraints" sheetId="7" r:id="rId7"/>
-    <sheet name="Heavy Feeder Constraints" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="120">
   <si>
     <t>Family</t>
   </si>
@@ -339,324 +334,18 @@
     <t>Broccoli (early season)</t>
   </si>
   <si>
-    <t>Constraint</t>
-  </si>
-  <si>
-    <t>Implement?</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Strictly?</t>
-  </si>
-  <si>
     <t>Field</t>
   </si>
   <si>
     <t>Crop</t>
   </si>
   <si>
-    <t>Variable Index</t>
-  </si>
-  <si>
-    <t>Meaning</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Model Variable</t>
-  </si>
-  <si>
-    <t>{0,1}</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Float</t>
-  </si>
-  <si>
-    <t>Unmet Demand  of Product m in year k</t>
-  </si>
-  <si>
-    <t>Crop (Crops.Plant)</t>
-  </si>
-  <si>
-    <t>Field (Farmland.Field)</t>
-  </si>
-  <si>
-    <t>Demand Crop/Product (Crops.Is same product as)</t>
-  </si>
-  <si>
-    <t>X_i_j_k_l</t>
-  </si>
-  <si>
-    <t>U_m_k</t>
-  </si>
-  <si>
-    <t>Type/Values</t>
-  </si>
-  <si>
-    <t>Land Use in field j</t>
-  </si>
-  <si>
-    <t>Field j available land in year k month l</t>
-  </si>
-  <si>
-    <t>Field j available land in year k month l+1</t>
-  </si>
-  <si>
-    <t>RHS</t>
-  </si>
-  <si>
-    <t>=</t>
-  </si>
-  <si>
-    <t>X_i+1_j_k_l</t>
-  </si>
-  <si>
-    <t>L_j_k_l</t>
-  </si>
-  <si>
-    <t>Unused land of field j in year k month l</t>
-  </si>
-  <si>
-    <t>-1</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>+1</t>
-  </si>
-  <si>
-    <t>Field j available land in year k month l+2</t>
-  </si>
-  <si>
-    <t>X_i_j_j_l+1</t>
-  </si>
-  <si>
-    <t>X_i+1_j_k_l+1</t>
-  </si>
-  <si>
-    <t>L_j_k_l+1</t>
-  </si>
-  <si>
-    <t>To initialize set the RHS to available land of field j</t>
-  </si>
-  <si>
-    <t>Crop i planted on j in year k month l (bed feet)</t>
-  </si>
-  <si>
-    <t>Crop i+1 planted on j in year k month l (bed feet)</t>
-  </si>
-  <si>
-    <t>Field j land not used in year k month l (bed feet)</t>
-  </si>
-  <si>
-    <t>Crop I planted on j in year k month l+1 (bed feet)</t>
-  </si>
-  <si>
-    <t>Crop i+1 planted on j in year k month l+1 (bed feet)</t>
-  </si>
-  <si>
-    <t>Field j land not used in year k month l+1 (bed feet)</t>
-  </si>
-  <si>
-    <t>Field j available land in year k month l+3</t>
-  </si>
-  <si>
-    <t>Field j available land in year k month l+4</t>
-  </si>
-  <si>
-    <t>Field j available land in year k month l+5</t>
-  </si>
-  <si>
-    <t>Field j available land in year k month l+6</t>
-  </si>
-  <si>
-    <t>Field j available land in year k month l+7</t>
-  </si>
-  <si>
-    <t>Field j available land in year k month l+8</t>
-  </si>
-  <si>
-    <t>Field j available land in year k month l+9</t>
-  </si>
-  <si>
-    <t>Field j available land in year k month l+10</t>
-  </si>
-  <si>
-    <t>Field j available land in year k month l+11</t>
-  </si>
-  <si>
-    <t>Crop i planted on j in year k month l (bed feet) harvested; it releases the land (120 days to maturity)</t>
-  </si>
-  <si>
-    <t>Crop i+1 planted on j in year k month l (bed feet) harvested; it releases the land (75 days to maturity)</t>
-  </si>
-  <si>
-    <t>X_i_j_j_l+4</t>
-  </si>
-  <si>
-    <t>X_i+1_j_k_l+4</t>
-  </si>
-  <si>
-    <t>L_j_k_l+4</t>
-  </si>
-  <si>
-    <t>Crop i planted on j in year k month l+4 (bed feet)</t>
-  </si>
-  <si>
-    <t>Crop i+1 planted on j in year k month l+4 (bed feet)</t>
-  </si>
-  <si>
-    <t>Field j land not used in year k month l+4 (bed feet)</t>
-  </si>
-  <si>
-    <t>Field j available land in year k+1 month l</t>
-  </si>
-  <si>
-    <t>XP_i_j_k_l</t>
-  </si>
-  <si>
-    <t>{0,1} = 1 if Crop i planted on j in year k month l</t>
-  </si>
-  <si>
-    <t>XP_i+1_j_k_l</t>
-  </si>
-  <si>
-    <t>{0,1} = 1 if Crop i+1 planted on j in year k month l</t>
-  </si>
-  <si>
-    <t>=1 if crop i is planted in field j in month l of year k</t>
-  </si>
-  <si>
-    <t>Row Feet of crop i planted in field j in month l of year k</t>
-  </si>
-  <si>
-    <t>&gt;=</t>
-  </si>
-  <si>
-    <t>Minimum feet of field j planted to crop i in year k month l</t>
-  </si>
-  <si>
-    <t>Minimum feet of field j planted to crop i+1 in year k month l</t>
-  </si>
-  <si>
-    <t>Constant</t>
-  </si>
-  <si>
-    <t>MPF_j</t>
-  </si>
-  <si>
-    <t>-MPF_j</t>
-  </si>
-  <si>
-    <t>Minimum Planted Feet of Field j (Farmland.Minimum Planting Feet (MPF_j))</t>
-  </si>
-  <si>
-    <t>Minimum Planted Feet</t>
-  </si>
-  <si>
-    <t>The number of feet that have to be planted in a field (must be less than the length of the field but it's engouraged to be the entire length of the field)</t>
-  </si>
-  <si>
-    <t>BAF_j</t>
-  </si>
-  <si>
-    <t>Is Same Crop As (SCA)</t>
-  </si>
-  <si>
-    <t>Yearly Demand (lbs) (SCAD)</t>
-  </si>
-  <si>
-    <t>Unmet demand of crop m in year k</t>
-  </si>
-  <si>
-    <t>U_m+1_k</t>
-  </si>
-  <si>
-    <t>Unmet demand of crop m+1 in year k</t>
-  </si>
-  <si>
-    <t>XY_i_j_k_l</t>
-  </si>
-  <si>
-    <t>Yield per unit of bed of crop I planted in field j in month l of year k</t>
-  </si>
-  <si>
-    <t>SCAD_m_k</t>
-  </si>
-  <si>
-    <t>Demand of crop m in year k</t>
-  </si>
-  <si>
-    <t>SCA_m</t>
-  </si>
-  <si>
-    <t>+XY_i_j_k_l</t>
-  </si>
-  <si>
-    <t>Crop i planted on j in year k month l+1 (bed feet)</t>
-  </si>
-  <si>
-    <t>Demand</t>
-  </si>
-  <si>
-    <t>Unmet demand of (same as) crop m in year k equals demand minus yield*bed feet planted</t>
-  </si>
-  <si>
-    <t>Heavy Feeder Crop Land Release in field j</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>Heavy Feeder Crop i planted on j in year k month l (bed feet) harvested; it releases the land (120 days to maturity)</t>
-  </si>
-  <si>
-    <t>Constraint Implemented elsewhere</t>
-  </si>
-  <si>
-    <t>{0,1} = 1 if Heavy Feeder Crop i planted on j in year k month l released land in year k month l+4</t>
-  </si>
-  <si>
-    <t>XH_i_j_k_l(+4)</t>
-  </si>
-  <si>
     <t>Years between plantings on same field</t>
   </si>
   <si>
     <t>Include?</t>
   </si>
   <si>
-    <t>PH</t>
-  </si>
-  <si>
-    <t>BFA_j</t>
-  </si>
-  <si>
-    <t>Planning horizon: number of years to plan for (must be 1 or greater)</t>
-  </si>
-  <si>
     <t>Measure</t>
   </si>
   <si>
@@ -694,6 +383,9 @@
   </si>
   <si>
     <t>Row 10</t>
+  </si>
+  <si>
+    <t>Yearly Demand</t>
   </si>
 </sst>
 </file>
@@ -743,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -778,28 +470,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -807,6 +481,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1112,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1124,24 +801,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>208</v>
-      </c>
       <c r="C1" s="10" t="s">
-        <v>209</v>
+        <v>107</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>204</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="C2">
         <v>25</v>
@@ -1152,10 +829,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>25</v>
@@ -1166,10 +843,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="C4">
         <v>25</v>
@@ -1180,10 +857,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="C5">
         <v>25</v>
@@ -1194,10 +871,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="C6">
         <v>25</v>
@@ -1208,10 +885,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="C7">
         <v>25</v>
@@ -1222,10 +899,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="C8">
         <v>25</v>
@@ -1236,10 +913,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>218</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="C9">
         <v>25</v>
@@ -1250,10 +927,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>219</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="C10">
         <v>25</v>
@@ -1264,10 +941,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>220</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="C11">
         <v>25</v>
@@ -1328,28 +1005,28 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
-      <c r="I1" s="16"/>
+      <c r="I1" s="13"/>
       <c r="J1" s="11"/>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
       <c r="W1" s="11"/>
       <c r="X1" s="11"/>
     </row>
     <row r="2" spans="1:24" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>0</v>
@@ -1373,7 +1050,7 @@
         <v>22</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>25</v>
@@ -2542,7 +2219,7 @@
       <c r="H24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="20"/>
+      <c r="I24" s="14"/>
       <c r="J24" s="5">
         <v>1.5</v>
       </c>
@@ -3415,7 +3092,7 @@
       <c r="A41" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="12" t="s">
         <v>79</v>
       </c>
       <c r="C41" s="6" t="s">
@@ -3719,26 +3396,26 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="8" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>183</v>
+        <v>33</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>184</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="8">
@@ -3754,7 +3431,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="8">
@@ -3814,848 +3491,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.33203125" style="2"/>
-    <col min="2" max="2" width="23.21875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="8"/>
-    <col min="4" max="4" width="11.33203125" style="17"/>
-    <col min="5" max="5" width="13.44140625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="55.77734375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="8"/>
-    <col min="8" max="8" width="17.33203125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="39.6640625" style="8" customWidth="1"/>
-    <col min="10" max="16384" width="11.33203125" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="123.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O19"/>
-  <sheetViews>
-    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N5" sqref="N5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.6640625" style="8" customWidth="1"/>
-    <col min="2" max="12" width="16" style="8" customWidth="1"/>
-    <col min="13" max="13" width="5.44140625" style="8" customWidth="1"/>
-    <col min="14" max="14" width="6.5546875" style="8" customWidth="1"/>
-    <col min="15" max="15" width="47.5546875" style="8" customWidth="1"/>
-    <col min="16" max="16384" width="18" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="N5" s="15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="M7" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="N7" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="N8" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="O8" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="N9" s="15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-    </row>
-    <row r="18" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="M18" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="N18" s="15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="L19" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="M19" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="N19" s="15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.6640625" style="8" customWidth="1"/>
-    <col min="2" max="9" width="16" style="8" customWidth="1"/>
-    <col min="10" max="10" width="5.44140625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="11" style="8" customWidth="1"/>
-    <col min="12" max="12" width="47.5546875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="18" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>196</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.6640625" style="8" customWidth="1"/>
-    <col min="2" max="6" width="16" style="8" customWidth="1"/>
-    <col min="7" max="7" width="23" style="8" customWidth="1"/>
-    <col min="8" max="8" width="5.44140625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" style="8" customWidth="1"/>
-    <col min="10" max="10" width="49.33203125" style="8" customWidth="1"/>
-    <col min="11" max="11" width="21.6640625" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="18" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-    </row>
-    <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F11" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Started code to prepare the model from the data read from the spreadsheet
</commit_message>
<xml_diff>
--- a/data/Crop Rotation Sample Template.xlsx
+++ b/data/Crop Rotation Sample Template.xlsx
@@ -964,10 +964,10 @@
   <dimension ref="A1:X46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomRight" activeCell="X31" sqref="X31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1354,7 +1354,7 @@
         <v>80</v>
       </c>
       <c r="X7" s="6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1406,7 +1406,7 @@
         <v>80</v>
       </c>
       <c r="X8" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1611,7 +1611,7 @@
         <v>120</v>
       </c>
       <c r="X12" s="6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2029,7 +2029,7 @@
         <v>120</v>
       </c>
       <c r="X20" s="6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2610,7 +2610,7 @@
         <v>120</v>
       </c>
       <c r="X31" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.3">
@@ -2873,7 +2873,7 @@
         <v>60</v>
       </c>
       <c r="X36" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.3">
@@ -2929,7 +2929,7 @@
         <v>80</v>
       </c>
       <c r="X37" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.3">
@@ -2985,7 +2985,7 @@
         <v>130</v>
       </c>
       <c r="X38" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.3">
@@ -3282,7 +3282,7 @@
         <v>120</v>
       </c>
       <c r="X44" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added more model variables.
</commit_message>
<xml_diff>
--- a/data/Crop Rotation Sample Template.xlsx
+++ b/data/Crop Rotation Sample Template.xlsx
@@ -337,9 +337,6 @@
     <t>Crop</t>
   </si>
   <si>
-    <t>Years between plantings on same field</t>
-  </si>
-  <si>
     <t>Include?</t>
   </si>
   <si>
@@ -386,6 +383,9 @@
   </si>
   <si>
     <t>Yield per Unit of Field</t>
+  </si>
+  <si>
+    <t>Months between plantings on same field</t>
   </si>
 </sst>
 </file>
@@ -804,21 +804,21 @@
         <v>101</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>106</v>
-      </c>
       <c r="D1" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2">
         <v>25</v>
@@ -829,10 +829,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3">
         <v>25</v>
@@ -843,10 +843,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C4">
         <v>25</v>
@@ -857,10 +857,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5">
         <v>25</v>
@@ -871,10 +871,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6">
         <v>25</v>
@@ -885,10 +885,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7">
         <v>25</v>
@@ -899,10 +899,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8">
         <v>25</v>
@@ -913,10 +913,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9">
         <v>25</v>
@@ -927,10 +927,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10">
         <v>25</v>
@@ -941,10 +941,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11">
         <v>25</v>
@@ -964,10 +964,10 @@
   <dimension ref="A1:X46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X31" sqref="X31"/>
+      <selection pane="bottomRight" activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1024,7 +1024,7 @@
       <c r="W1" s="11"/>
       <c r="X1" s="11"/>
     </row>
-    <row r="2" spans="1:24" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>102</v>
       </c>
@@ -1050,10 +1050,10 @@
         <v>22</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>1</v>
@@ -1329,7 +1329,7 @@
         <v>18</v>
       </c>
       <c r="I7" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="J7" s="5">
         <v>0.5</v>
@@ -1383,7 +1383,7 @@
         <v>18</v>
       </c>
       <c r="I8" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="J8" s="5">
         <v>0.5</v>
@@ -1435,7 +1435,7 @@
         <v>18</v>
       </c>
       <c r="I9" s="3">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="J9" s="5">
         <v>0.5</v>
@@ -1640,7 +1640,7 @@
         <v>18</v>
       </c>
       <c r="I13" s="3">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="J13" s="5">
         <v>1</v>
@@ -1694,7 +1694,7 @@
         <v>18</v>
       </c>
       <c r="I14" s="3">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="J14" s="5">
         <v>1</v>
@@ -1848,7 +1848,7 @@
         <v>18</v>
       </c>
       <c r="I17" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="J17" s="5">
         <v>0.7</v>
@@ -1902,7 +1902,7 @@
         <v>18</v>
       </c>
       <c r="I18" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="J18" s="5">
         <v>0.7</v>
@@ -2058,7 +2058,7 @@
         <v>18</v>
       </c>
       <c r="I21" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="J21" s="5">
         <v>0.7</v>
@@ -2112,7 +2112,7 @@
         <v>18</v>
       </c>
       <c r="I22" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="J22" s="5">
         <v>0.7</v>
@@ -2583,7 +2583,7 @@
         <v>18</v>
       </c>
       <c r="I31" s="3">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="J31" s="5">
         <v>0.25</v>
@@ -2788,7 +2788,7 @@
         <v>18</v>
       </c>
       <c r="I35" s="3">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="J35" s="5">
         <v>1.2</v>
@@ -2846,7 +2846,7 @@
         <v>18</v>
       </c>
       <c r="I36" s="3">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="J36" s="5">
         <v>2</v>
@@ -2902,7 +2902,7 @@
         <v>18</v>
       </c>
       <c r="I37" s="3">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="J37" s="5">
         <v>2</v>
@@ -2958,7 +2958,7 @@
         <v>18</v>
       </c>
       <c r="I38" s="3">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="J38" s="5">
         <v>2</v>
@@ -3411,7 +3411,7 @@
         <v>32</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
begin teting with multiple year data
</commit_message>
<xml_diff>
--- a/data/Crop Rotation Sample Template.xlsx
+++ b/data/Crop Rotation Sample Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9312" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9312" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Farmland" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="120">
   <si>
     <t>Family</t>
   </si>
@@ -376,9 +376,6 @@
     <t>Row 9</t>
   </si>
   <si>
-    <t>Row 10</t>
-  </si>
-  <si>
     <t>Yearly Demand</t>
   </si>
   <si>
@@ -386,6 +383,9 @@
   </si>
   <si>
     <t>Months between plantings on same field</t>
+  </si>
+  <si>
+    <t>Row A</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -485,11 +485,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -790,7 +800,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -852,7 +862,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -866,7 +876,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -880,7 +890,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -894,7 +904,7 @@
         <v>25</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -908,7 +918,7 @@
         <v>25</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -922,7 +932,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -936,12 +946,12 @@
         <v>25</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
         <v>106</v>
@@ -950,7 +960,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -963,11 +973,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I41" sqref="I41"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,10 +1060,10 @@
         <v>22</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>1</v>
@@ -1354,7 +1364,7 @@
         <v>80</v>
       </c>
       <c r="X7" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1406,7 +1416,7 @@
         <v>80</v>
       </c>
       <c r="X8" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1462,7 +1472,7 @@
         <v>155</v>
       </c>
       <c r="X9" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1665,7 +1675,7 @@
         <v>100</v>
       </c>
       <c r="X13" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2929,7 +2939,7 @@
         <v>80</v>
       </c>
       <c r="X37" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.3">
@@ -2985,7 +2995,7 @@
         <v>130</v>
       </c>
       <c r="X38" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.3">
@@ -3034,7 +3044,7 @@
         <v>110</v>
       </c>
       <c r="X39" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.3">
@@ -3282,7 +3292,7 @@
         <v>120</v>
       </c>
       <c r="X44" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.3">
@@ -3382,7 +3392,7 @@
     <mergeCell ref="K1:V1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:X46">
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3393,10 +3403,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3411,7 +3421,7 @@
         <v>32</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3431,55 +3441,84 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
-        <v>33</v>
+      <c r="A4" s="17" t="s">
+        <v>34</v>
       </c>
       <c r="B4" s="8">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B5" s="8">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B6" s="8">
-        <v>150</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>69</v>
+      <c r="A7" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="B7" s="8">
-        <v>250</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B8" s="8">
-        <v>20</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="8">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B10" s="8">
         <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="8">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Still working on rotation constraints
</commit_message>
<xml_diff>
--- a/data/Crop Rotation Sample Template.xlsx
+++ b/data/Crop Rotation Sample Template.xlsx
@@ -9,13 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9312" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9312" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Farmland" sheetId="3" r:id="rId1"/>
     <sheet name="Crops" sheetId="1" r:id="rId2"/>
     <sheet name="Demand" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Crops!$A$2:$X$46</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -482,11 +485,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -971,9 +974,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1017,20 +1021,20 @@
       <c r="H1" s="11"/>
       <c r="I1" s="13"/>
       <c r="J1" s="11"/>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
       <c r="W1" s="11"/>
       <c r="X1" s="11"/>
     </row>
@@ -1108,7 +1112,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -1158,7 +1162,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>92</v>
       </c>
@@ -1261,7 +1265,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -1475,7 +1479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>96</v>
       </c>
@@ -1524,7 +1528,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>94</v>
       </c>
@@ -1575,7 +1579,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -1678,7 +1682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1730,7 +1734,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -1782,7 +1786,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
@@ -1832,7 +1836,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:24" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" s="5" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>43</v>
       </c>
@@ -1886,7 +1890,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:24" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" s="5" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>50</v>
       </c>
@@ -1938,7 +1942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:24" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" s="5" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
@@ -1990,7 +1994,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:24" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" s="5" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>48</v>
       </c>
@@ -2042,7 +2046,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>51</v>
       </c>
@@ -2096,7 +2100,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>55</v>
       </c>
@@ -2150,7 +2154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>56</v>
       </c>
@@ -2204,7 +2208,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>53</v>
       </c>
@@ -2256,7 +2260,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>54</v>
       </c>
@@ -2308,7 +2312,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>58</v>
       </c>
@@ -2360,7 +2364,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>60</v>
       </c>
@@ -2412,7 +2416,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>62</v>
       </c>
@@ -2464,7 +2468,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>63</v>
       </c>
@@ -2516,7 +2520,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>93</v>
       </c>
@@ -2567,7 +2571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>66</v>
       </c>
@@ -2623,7 +2627,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>75</v>
       </c>
@@ -2674,7 +2678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>76</v>
       </c>
@@ -2723,7 +2727,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>67</v>
       </c>
@@ -2772,7 +2776,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>68</v>
       </c>
@@ -2830,7 +2834,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>70</v>
       </c>
@@ -3047,7 +3051,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>90</v>
       </c>
@@ -3098,7 +3102,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>77</v>
       </c>
@@ -3148,7 +3152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>80</v>
       </c>
@@ -3295,7 +3299,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>87</v>
       </c>
@@ -3336,7 +3340,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>89</v>
       </c>
@@ -3388,6 +3392,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:X46">
+    <filterColumn colId="23">
+      <filters>
+        <filter val="Y"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="K1:V1"/>
   </mergeCells>
@@ -3405,7 +3416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3441,7 +3452,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="8">

</xml_diff>

<commit_message>
Rounds of testing in association with Python development
</commit_message>
<xml_diff>
--- a/data/Crop Rotation Sample Template.xlsx
+++ b/data/Crop Rotation Sample Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9312" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9312"/>
   </bookViews>
   <sheets>
     <sheet name="Farmland" sheetId="3" r:id="rId1"/>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1529,7 +1529,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>